<commit_message>
Atualização no ppt e algumas documentações
</commit_message>
<xml_diff>
--- a/_Projeto-Estagio_/Projeto/documentacao/Documentos/Backlog.xlsx
+++ b/_Projeto-Estagio_/Projeto/documentacao/Documentos/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\René\Desktop\_Vitor\_Faculdade\_Estagio_\Estagio\_Projeto-Estagio_\Projeto\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Faculdade\_Estagio_\estagio\Estagio\_Projeto-Estagio_\Projeto\documentacao\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>ID_ENTREGA</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Concluído</t>
   </si>
   <si>
-    <t>Andamento</t>
-  </si>
-  <si>
     <t>Montar modelo lógico do banco</t>
   </si>
   <si>
@@ -114,6 +111,12 @@
   </si>
   <si>
     <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>Fazer BPMN da aplicação</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="A2:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -559,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -576,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -593,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -618,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>17</v>
@@ -633,7 +636,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -648,10 +651,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>17</v>
@@ -665,10 +668,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>17</v>
@@ -682,10 +685,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>17</v>
@@ -698,7 +701,21 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="9">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>

</xml_diff>